<commit_message>
added iframe to readme
</commit_message>
<xml_diff>
--- a/Originals/classroom_tech_room_updates.xlsx
+++ b/Originals/classroom_tech_room_updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/repos/Classroom-Technology/Originals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A070C823-A33F-294B-A0A4-6895B5BF12CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F474C0FD-1B1D-684C-B790-6B822A7DD38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21000" xr2:uid="{20F71E7D-4287-49C5-8E90-ED4F0DDD2463}"/>
+    <workbookView xWindow="2480" yWindow="1160" windowWidth="26240" windowHeight="16400" xr2:uid="{20F71E7D-4287-49C5-8E90-ED4F0DDD2463}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1156,20 +1156,20 @@
   <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
-    <col min="7" max="7" width="47.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1203,128 +1203,128 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F2" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F3" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F4" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F5" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>192</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>244</v>
@@ -1333,67 +1333,67 @@
         <v>231</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>194</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>195</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>244</v>
@@ -1402,21 +1402,21 @@
         <v>231</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>196</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>244</v>
@@ -1425,44 +1425,44 @@
         <v>231</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>244</v>
@@ -1471,165 +1471,165 @@
         <v>231</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F16" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>18</v>
+        <v>203</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F17" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F18" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F19" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="G19" t="s">
-        <v>184</v>
+        <v>23</v>
       </c>
       <c r="H19" t="s">
-        <v>185</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
         <v>182</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F20" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="G20" t="s">
         <v>184</v>
@@ -1640,19 +1640,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B21" t="s">
         <v>182</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F21" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="G21" t="s">
         <v>184</v>
@@ -1669,7 +1669,7 @@
         <v>182</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>244</v>
@@ -1689,10 +1689,10 @@
         <v>199</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>244</v>
@@ -1701,286 +1701,286 @@
         <v>202</v>
       </c>
       <c r="G23" t="s">
-        <v>184</v>
+        <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>185</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F24" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="G24" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="H24" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>115</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F25" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="G25" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
-        <v>185</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>192</v>
+        <v>11</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G26" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G27" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>194</v>
+        <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G28" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>195</v>
+        <v>18</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G29" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>19</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>196</v>
+        <v>20</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G30" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>210</v>
+        <v>22</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F31" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G31" t="s">
-        <v>184</v>
+        <v>23</v>
       </c>
       <c r="H31" t="s">
-        <v>185</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G32" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>197</v>
+        <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G33" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>198</v>
+        <v>28</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G34" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>183</v>
+        <v>30</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G35" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1988,10 +1988,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>244</v>
@@ -2000,21 +2000,21 @@
         <v>230</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>244</v>
@@ -2023,33 +2023,33 @@
         <v>230</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G38" t="s">
-        <v>237</v>
+        <v>33</v>
       </c>
       <c r="H38" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>236</v>
@@ -2057,13 +2057,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>244</v>
@@ -2080,42 +2080,42 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H40" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G41" t="s">
         <v>12</v>
@@ -2126,19 +2126,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G42" t="s">
         <v>12</v>
@@ -2149,13 +2149,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>244</v>
@@ -2164,21 +2164,21 @@
         <v>230</v>
       </c>
       <c r="G43" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="H43" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>244</v>
@@ -2187,21 +2187,21 @@
         <v>230</v>
       </c>
       <c r="G44" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>244</v>
@@ -2210,21 +2210,21 @@
         <v>230</v>
       </c>
       <c r="G45" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="H45" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>244</v>
@@ -2233,21 +2233,21 @@
         <v>230</v>
       </c>
       <c r="G46" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>244</v>
@@ -2264,13 +2264,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B48" t="s">
         <v>56</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>244</v>
@@ -2279,10 +2279,10 @@
         <v>230</v>
       </c>
       <c r="G48" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -2293,7 +2293,7 @@
         <v>56</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>244</v>
@@ -2310,13 +2310,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>244</v>
@@ -2325,21 +2325,21 @@
         <v>230</v>
       </c>
       <c r="G50" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="H50" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>244</v>
@@ -2348,160 +2348,160 @@
         <v>230</v>
       </c>
       <c r="G51" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>233</v>
+        <v>63</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F52" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="G52" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G53" t="s">
-        <v>238</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>239</v>
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
+        <v>13</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F54" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G54" t="s">
-        <v>238</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>239</v>
+        <v>68</v>
+      </c>
+      <c r="H54" t="s">
+        <v>69</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F55" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G55" t="s">
-        <v>238</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>239</v>
+        <v>68</v>
+      </c>
+      <c r="H55" t="s">
+        <v>69</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F56" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G56" t="s">
-        <v>238</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>239</v>
+        <v>68</v>
+      </c>
+      <c r="H56" t="s">
+        <v>69</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F57" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G57" t="s">
-        <v>238</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>239</v>
+        <v>68</v>
+      </c>
+      <c r="H57" t="s">
+        <v>69</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>240</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>244</v>
@@ -2524,21 +2524,21 @@
         <v>230</v>
       </c>
       <c r="G58" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H58" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>244</v>
@@ -2547,21 +2547,21 @@
         <v>230</v>
       </c>
       <c r="G59" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H59" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>244</v>
@@ -2578,19 +2578,19 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F61" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G61" t="s">
         <v>12</v>
@@ -2604,22 +2604,22 @@
         <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G62" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H62" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -2627,10 +2627,10 @@
         <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>244</v>
@@ -2650,10 +2650,10 @@
         <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>244</v>
@@ -2670,25 +2670,25 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>199</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>211</v>
+        <v>83</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F65" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="G65" t="s">
-        <v>212</v>
+        <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>213</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2696,10 +2696,10 @@
         <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>244</v>
@@ -2719,19 +2719,22 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>229</v>
+        <v>85</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F67" t="s">
+        <v>230</v>
+      </c>
       <c r="G67" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H67" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2739,10 +2742,10 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>244</v>
@@ -2751,10 +2754,10 @@
         <v>231</v>
       </c>
       <c r="G68" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="H68" t="s">
-        <v>13</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2762,10 +2765,10 @@
         <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>244</v>
@@ -2785,10 +2788,10 @@
         <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>244</v>
@@ -2808,22 +2811,22 @@
         <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F71" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G71" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H71" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2831,22 +2834,22 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G72" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H72" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2854,22 +2857,22 @@
         <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F73" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G73" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H73" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2877,19 +2880,22 @@
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>214</v>
+        <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F74" t="s">
+        <v>230</v>
+      </c>
       <c r="G74" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H74" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2897,10 +2903,10 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>244</v>
@@ -2909,10 +2915,10 @@
         <v>230</v>
       </c>
       <c r="G75" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H75" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2920,22 +2926,22 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G76" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H76" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2943,137 +2949,137 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F77" t="s">
+        <v>230</v>
+      </c>
+      <c r="G77" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>96</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F78" t="s">
         <v>231</v>
       </c>
-      <c r="G77" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78" t="s">
-        <v>115</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F78" t="s">
-        <v>230</v>
-      </c>
       <c r="G78" t="s">
-        <v>60</v>
-      </c>
-      <c r="H78" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F79" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G79" t="s">
-        <v>60</v>
-      </c>
-      <c r="H79" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>234</v>
+        <v>99</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F80" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G80" t="s">
-        <v>60</v>
-      </c>
-      <c r="H80" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F81" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="G81" t="s">
-        <v>60</v>
-      </c>
-      <c r="H81" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F82" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G82" t="s">
-        <v>12</v>
-      </c>
-      <c r="H82" t="s">
-        <v>13</v>
+        <v>238</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3081,16 +3087,16 @@
         <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F83" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G83" t="s">
         <v>12</v>
@@ -3104,16 +3110,16 @@
         <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F84" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G84" t="s">
         <v>12</v>
@@ -3124,19 +3130,19 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F85" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G85" t="s">
         <v>12</v>
@@ -3147,13 +3153,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>244</v>
@@ -3162,10 +3168,10 @@
         <v>230</v>
       </c>
       <c r="G86" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H86" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>35</v>
@@ -3176,22 +3182,19 @@
         <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>123</v>
+        <v>229</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F87" t="s">
-        <v>230</v>
-      </c>
       <c r="G87" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H87" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>35</v>
@@ -3202,22 +3205,22 @@
         <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F88" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G88" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H88" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>35</v>
@@ -3228,22 +3231,22 @@
         <v>78</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F89" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G89" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H89" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>35</v>
@@ -3251,25 +3254,25 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F90" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G90" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H90" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>35</v>
@@ -3277,13 +3280,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>244</v>
@@ -3292,10 +3295,10 @@
         <v>230</v>
       </c>
       <c r="G91" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H91" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>35</v>
@@ -3306,16 +3309,16 @@
         <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F92" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G92" t="s">
         <v>12</v>
@@ -3329,16 +3332,16 @@
         <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F93" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G93" t="s">
         <v>12</v>
@@ -3349,19 +3352,16 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>39</v>
+        <v>214</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F94" t="s">
-        <v>230</v>
       </c>
       <c r="G94" t="s">
         <v>12</v>
@@ -3375,10 +3375,10 @@
         <v>78</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>244</v>
@@ -3387,27 +3387,27 @@
         <v>230</v>
       </c>
       <c r="G95" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H95" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F96" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G96" t="s">
         <v>12</v>
@@ -3421,16 +3421,16 @@
         <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F97" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G97" t="s">
         <v>12</v>
@@ -3444,10 +3444,10 @@
         <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>244</v>
@@ -3456,10 +3456,10 @@
         <v>230</v>
       </c>
       <c r="G98" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H98" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -3467,19 +3467,22 @@
         <v>78</v>
       </c>
       <c r="B99" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>224</v>
+        <v>117</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F99" t="s">
+        <v>230</v>
+      </c>
       <c r="G99" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H99" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -3487,19 +3490,22 @@
         <v>78</v>
       </c>
       <c r="B100" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F100" t="s">
+        <v>230</v>
+      </c>
       <c r="G100" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H100" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -3507,13 +3513,16 @@
         <v>78</v>
       </c>
       <c r="B101" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>226</v>
+        <v>120</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>244</v>
+      </c>
+      <c r="F101" t="s">
+        <v>230</v>
       </c>
       <c r="G101" t="s">
         <v>12</v>
@@ -3527,13 +3536,16 @@
         <v>78</v>
       </c>
       <c r="B102" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>227</v>
+        <v>121</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>244</v>
+      </c>
+      <c r="F102" t="s">
+        <v>230</v>
       </c>
       <c r="G102" t="s">
         <v>12</v>
@@ -3547,10 +3559,10 @@
         <v>78</v>
       </c>
       <c r="B103" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>244</v>
@@ -3570,10 +3582,10 @@
         <v>78</v>
       </c>
       <c r="B104" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>244</v>
@@ -3582,10 +3594,10 @@
         <v>230</v>
       </c>
       <c r="G104" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H104" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -3593,22 +3605,22 @@
         <v>78</v>
       </c>
       <c r="B105" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F105" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G105" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H105" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -3616,10 +3628,10 @@
         <v>78</v>
       </c>
       <c r="B106" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>244</v>
@@ -3628,10 +3640,10 @@
         <v>230</v>
       </c>
       <c r="G106" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H106" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
@@ -3639,13 +3651,16 @@
         <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>228</v>
+        <v>127</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>244</v>
+      </c>
+      <c r="F107" t="s">
+        <v>230</v>
       </c>
       <c r="G107" t="s">
         <v>12</v>
@@ -3656,25 +3671,25 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B108" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F108" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G108" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>70</v>
@@ -3682,25 +3697,25 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F109" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G109" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H109" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>70</v>
@@ -3708,25 +3723,25 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B110" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F110" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G110" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H110" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>70</v>
@@ -3737,22 +3752,22 @@
         <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F111" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G111" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H111" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>70</v>
@@ -3763,22 +3778,19 @@
         <v>78</v>
       </c>
       <c r="B112" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>137</v>
+        <v>224</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F112" t="s">
-        <v>232</v>
-      </c>
       <c r="G112" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H112" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>70</v>
@@ -3786,25 +3798,22 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B113" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F113" t="s">
-        <v>232</v>
-      </c>
       <c r="G113" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H113" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>70</v>
@@ -3815,22 +3824,19 @@
         <v>78</v>
       </c>
       <c r="B114" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>138</v>
+        <v>226</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F114" t="s">
-        <v>230</v>
-      </c>
       <c r="G114" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H114" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>35</v>
@@ -3841,22 +3847,19 @@
         <v>78</v>
       </c>
       <c r="B115" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>139</v>
+        <v>227</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F115" t="s">
-        <v>230</v>
-      </c>
       <c r="G115" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H115" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>35</v>
@@ -3864,13 +3867,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B116" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>244</v>
@@ -3879,10 +3882,10 @@
         <v>230</v>
       </c>
       <c r="G116" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H116" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>35</v>
@@ -3893,10 +3896,10 @@
         <v>78</v>
       </c>
       <c r="B117" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>244</v>
@@ -3905,10 +3908,10 @@
         <v>230</v>
       </c>
       <c r="G117" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H117" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>35</v>
@@ -3919,22 +3922,22 @@
         <v>78</v>
       </c>
       <c r="B118" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F118" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G118" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H118" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>35</v>
@@ -3945,10 +3948,10 @@
         <v>78</v>
       </c>
       <c r="B119" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>244</v>
@@ -3957,10 +3960,10 @@
         <v>230</v>
       </c>
       <c r="G119" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H119" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>35</v>
@@ -3968,25 +3971,22 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B120" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>76</v>
+        <v>228</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F120" t="s">
-        <v>230</v>
-      </c>
       <c r="G120" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H120" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>35</v>
@@ -3997,22 +3997,22 @@
         <v>78</v>
       </c>
       <c r="B121" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F121" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G121" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="H121" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>35</v>
@@ -4020,36 +4020,36 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F122" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G122" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="H122" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>78</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>244</v>
@@ -4058,24 +4058,24 @@
         <v>230</v>
       </c>
       <c r="G123" t="s">
-        <v>241</v>
-      </c>
-      <c r="H123" s="4" t="s">
-        <v>243</v>
+        <v>33</v>
+      </c>
+      <c r="H123" t="s">
+        <v>34</v>
       </c>
       <c r="I123" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>78</v>
       </c>
       <c r="B124" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>244</v>
@@ -4084,10 +4084,10 @@
         <v>230</v>
       </c>
       <c r="G124" t="s">
-        <v>241</v>
-      </c>
-      <c r="H124" s="4" t="s">
-        <v>243</v>
+        <v>33</v>
+      </c>
+      <c r="H124" t="s">
+        <v>34</v>
       </c>
       <c r="I124" s="5" t="s">
         <v>242</v>
@@ -4098,22 +4098,22 @@
         <v>78</v>
       </c>
       <c r="B125" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F125" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G125" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H125" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -4121,19 +4121,22 @@
         <v>78</v>
       </c>
       <c r="B126" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F126" t="s">
+        <v>230</v>
+      </c>
       <c r="G126" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H126" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -4141,19 +4144,22 @@
         <v>78</v>
       </c>
       <c r="B127" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>216</v>
+        <v>142</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F127" t="s">
+        <v>230</v>
+      </c>
       <c r="G127" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H127" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -4161,25 +4167,25 @@
         <v>78</v>
       </c>
       <c r="B128" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F128" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G128" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H128" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>78</v>
       </c>
@@ -4187,19 +4193,22 @@
         <v>144</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>217</v>
+        <v>145</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="F129" t="s">
+        <v>230</v>
+      </c>
       <c r="G129" t="s">
-        <v>12</v>
-      </c>
-      <c r="H129" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="H129" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>78</v>
       </c>
@@ -4207,19 +4216,19 @@
         <v>144</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F130" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G130" t="s">
-        <v>12</v>
-      </c>
-      <c r="H130" t="s">
-        <v>13</v>
+        <v>241</v>
+      </c>
+      <c r="H130" s="4" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -4230,10 +4239,13 @@
         <v>144</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>244</v>
+      </c>
+      <c r="F131" t="s">
+        <v>231</v>
       </c>
       <c r="G131" t="s">
         <v>12</v>
@@ -4250,7 +4262,7 @@
         <v>144</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>244</v>
@@ -4270,13 +4282,10 @@
         <v>144</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>150</v>
+        <v>216</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F133" t="s">
-        <v>231</v>
       </c>
       <c r="G133" t="s">
         <v>12</v>
@@ -4293,10 +4302,13 @@
         <v>144</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>244</v>
+      </c>
+      <c r="F134" t="s">
+        <v>231</v>
       </c>
       <c r="G134" t="s">
         <v>12</v>
@@ -4313,7 +4325,7 @@
         <v>144</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>244</v>
@@ -4333,7 +4345,7 @@
         <v>144</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>244</v>
@@ -4356,13 +4368,10 @@
         <v>144</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F137" t="s">
-        <v>231</v>
       </c>
       <c r="G137" t="s">
         <v>12</v>
@@ -4379,13 +4388,10 @@
         <v>144</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>153</v>
+        <v>219</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F138" t="s">
-        <v>231</v>
       </c>
       <c r="G138" t="s">
         <v>12</v>
@@ -4402,10 +4408,13 @@
         <v>144</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>244</v>
+      </c>
+      <c r="F139" t="s">
+        <v>231</v>
       </c>
       <c r="G139" t="s">
         <v>12</v>
@@ -4422,7 +4431,7 @@
         <v>144</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>244</v>
@@ -4436,19 +4445,16 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B141" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>43</v>
+        <v>221</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F141" t="s">
-        <v>230</v>
       </c>
       <c r="G141" t="s">
         <v>12</v>
@@ -4462,10 +4468,10 @@
         <v>78</v>
       </c>
       <c r="B142" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>244</v>
@@ -4485,10 +4491,10 @@
         <v>78</v>
       </c>
       <c r="B143" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>244</v>
@@ -4505,19 +4511,19 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B144" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F144" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G144" t="s">
         <v>12</v>
@@ -4531,22 +4537,19 @@
         <v>78</v>
       </c>
       <c r="B145" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F145" t="s">
-        <v>230</v>
-      </c>
       <c r="G145" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H145" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -4554,22 +4557,19 @@
         <v>78</v>
       </c>
       <c r="B146" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>157</v>
+        <v>223</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F146" t="s">
-        <v>230</v>
-      </c>
       <c r="G146" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H146" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -4577,22 +4577,22 @@
         <v>78</v>
       </c>
       <c r="B147" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F147" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G147" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H147" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -4600,22 +4600,22 @@
         <v>78</v>
       </c>
       <c r="B148" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F148" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G148" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H148" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -4626,7 +4626,7 @@
         <v>44</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>244</v>
@@ -4635,10 +4635,10 @@
         <v>230</v>
       </c>
       <c r="G149" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H149" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -4649,7 +4649,7 @@
         <v>44</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>244</v>
@@ -4658,10 +4658,10 @@
         <v>230</v>
       </c>
       <c r="G150" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H150" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>44</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>244</v>
@@ -4681,10 +4681,10 @@
         <v>230</v>
       </c>
       <c r="G151" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H151" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -4695,7 +4695,7 @@
         <v>44</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>244</v>
@@ -4704,10 +4704,10 @@
         <v>230</v>
       </c>
       <c r="G152" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H152" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -4718,7 +4718,7 @@
         <v>44</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>244</v>
@@ -4741,7 +4741,7 @@
         <v>44</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>244</v>
@@ -4764,7 +4764,7 @@
         <v>44</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>244</v>
@@ -4781,13 +4781,13 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B156" t="s">
         <v>44</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>244</v>
@@ -4810,7 +4810,7 @@
         <v>44</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>244</v>
@@ -4819,10 +4819,10 @@
         <v>230</v>
       </c>
       <c r="G157" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H157" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -4833,7 +4833,7 @@
         <v>44</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>244</v>
@@ -4842,10 +4842,10 @@
         <v>230</v>
       </c>
       <c r="G158" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H158" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -4856,7 +4856,7 @@
         <v>44</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>244</v>
@@ -4865,10 +4865,10 @@
         <v>230</v>
       </c>
       <c r="G159" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H159" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -4879,7 +4879,7 @@
         <v>44</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>244</v>
@@ -4902,7 +4902,7 @@
         <v>44</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>244</v>
@@ -4911,10 +4911,10 @@
         <v>230</v>
       </c>
       <c r="G161" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H161" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
@@ -4925,7 +4925,7 @@
         <v>44</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>244</v>
@@ -4948,7 +4948,7 @@
         <v>44</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>244</v>
@@ -4957,10 +4957,10 @@
         <v>230</v>
       </c>
       <c r="G163" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H163" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
@@ -4971,7 +4971,7 @@
         <v>44</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>244</v>
@@ -4980,10 +4980,10 @@
         <v>230</v>
       </c>
       <c r="G164" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H164" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -4994,7 +4994,7 @@
         <v>44</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>244</v>
@@ -5017,7 +5017,7 @@
         <v>44</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>244</v>
@@ -5026,10 +5026,10 @@
         <v>230</v>
       </c>
       <c r="G166" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H166" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
@@ -5040,7 +5040,7 @@
         <v>44</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>244</v>
@@ -5057,13 +5057,13 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B168" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>47</v>
+        <v>175</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>244</v>
@@ -5072,10 +5072,10 @@
         <v>230</v>
       </c>
       <c r="G168" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="H168" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="I168" s="2" t="s">
         <v>50</v>
@@ -5083,13 +5083,13 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B169" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>51</v>
+        <v>176</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>244</v>
@@ -5098,10 +5098,10 @@
         <v>230</v>
       </c>
       <c r="G169" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="H169" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="I169" s="2" t="s">
         <v>50</v>
@@ -5109,13 +5109,13 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B170" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>244</v>
@@ -5124,10 +5124,10 @@
         <v>230</v>
       </c>
       <c r="G170" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="H170" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="I170" s="2" t="s">
         <v>50</v>
@@ -5186,7 +5186,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H172" xr:uid="{0D0CE671-E4E0-4F44-90EF-1EB75C84044E}"/>
+  <autoFilter ref="A1:H172" xr:uid="{0D0CE671-E4E0-4F44-90EF-1EB75C84044E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H172">
+      <sortCondition ref="A1:A172"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I172">
     <sortCondition ref="B2:B172"/>
     <sortCondition ref="C2:C172"/>

</xml_diff>